<commit_message>
new style for excel sheet
</commit_message>
<xml_diff>
--- a/files/users.xlsx
+++ b/files/users.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <si>
+    <t>Name of Employee</t>
+  </si>
   <si>
     <t>Monthly Base Net Salary Eur</t>
   </si>
@@ -97,10 +100,16 @@
     <t>Total without VAT</t>
   </si>
   <si>
-    <t xml:space="preserve">VAT 20% </t>
+    <t xml:space="preserve">VAT10% </t>
   </si>
   <si>
     <t>Total with VAT</t>
+  </si>
+  <si>
+    <t>Albi</t>
+  </si>
+  <si>
+    <t>Adem</t>
   </si>
 </sst>
 </file>
@@ -116,7 +125,8 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,12 +137,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -141,7 +158,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,13 +500,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AE3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="30" width="20" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="31" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,97 +598,198 @@
       <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
         <v>500</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>75079.16</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>446.9</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>40</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>25</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>40</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>15</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>48</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>21</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>98876.57</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>8690.963060686001</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>107567.5296833773</v>
       </c>
-      <c r="O2">
-        <v>98876.5666226913</v>
-      </c>
       <c r="P2">
-        <v>9393.273829155674</v>
+        <v>107567.5296833773</v>
       </c>
       <c r="Q2">
-        <v>1680.9016325857522</v>
+        <v>10218.915319920843</v>
       </c>
       <c r="R2">
-        <v>11074.175461741426</v>
+        <v>1828.6480046174142</v>
       </c>
       <c r="S2">
-        <v>14831.484993403694</v>
+        <v>12047.563324538258</v>
       </c>
       <c r="T2">
-        <v>1680.9016325857522</v>
+        <v>16135.129452506595</v>
       </c>
       <c r="U2">
-        <v>16512.386625989446</v>
+        <v>1828.6480046174142</v>
       </c>
       <c r="V2">
+        <v>17963.777457124008</v>
+      </c>
+      <c r="W2">
         <v>107567.5296833773</v>
       </c>
-      <c r="W2">
-        <v>8953.95366094987</v>
-      </c>
       <c r="X2">
-        <v>78848.4375</v>
+        <v>10083.77885883905</v>
       </c>
       <c r="Y2">
-        <v>648.3180192402565</v>
+        <v>85436.18749999999</v>
       </c>
       <c r="Z2">
-        <v>1020.2262482269917</v>
+        <v>702.484685906923</v>
       </c>
       <c r="AA2">
-        <v>91.82036234042926</v>
+        <v>1032.1600652894367</v>
       </c>
       <c r="AB2">
-        <v>1112.0466105674209</v>
+        <v>92.8944058760493</v>
       </c>
       <c r="AC2">
+        <v>1125.0544711654861</v>
+      </c>
+      <c r="AD2">
         <v>0</v>
       </c>
-      <c r="AD2">
-        <v>1112.0466105674209</v>
+      <c r="AE2">
+        <v>1125.0544711654861</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>520</v>
+      </c>
+      <c r="C3">
+        <v>78288.13</v>
+      </c>
+      <c r="D3">
+        <v>466</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>25</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>48</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>21</v>
+      </c>
+      <c r="M3">
+        <v>103102.67</v>
+      </c>
+      <c r="N3">
+        <v>9038.601583113443</v>
+      </c>
+      <c r="O3">
+        <v>112141.26837542401</v>
+      </c>
+      <c r="P3">
+        <v>112141.26837542401</v>
+      </c>
+      <c r="Q3">
+        <v>10653.420495665281</v>
+      </c>
+      <c r="R3">
+        <v>1906.4015623822083</v>
+      </c>
+      <c r="S3">
+        <v>12559.82205804749</v>
+      </c>
+      <c r="T3">
+        <v>16821.190256313603</v>
+      </c>
+      <c r="U3">
+        <v>1906.4015623822083</v>
+      </c>
+      <c r="V3">
+        <v>18727.59181869581</v>
+      </c>
+      <c r="W3">
+        <v>112141.26837542401</v>
+      </c>
+      <c r="X3">
+        <v>10678.364888805123</v>
+      </c>
+      <c r="Y3">
+        <v>88903.0814285714</v>
+      </c>
+      <c r="Z3">
+        <v>730.9906382878753</v>
+      </c>
+      <c r="AA3">
+        <v>1076.0471977809557</v>
+      </c>
+      <c r="AB3">
+        <v>96.84424780028601</v>
+      </c>
+      <c r="AC3">
+        <v>1172.8914455812417</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>1172.8914455812417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>